<commit_message>
updated dictionary.csv and progess
</commit_message>
<xml_diff>
--- a/designs/i18n-de/i18n-de-progress.xlsx
+++ b/designs/i18n-de/i18n-de-progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\heikokue-node-red-designs\designs\i18n-de\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{56D5C65D-9282-42F0-B5A7-90EC9D91A72E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0913CC-B74F-44F4-A60C-E95A01C18E0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="-120" windowWidth="49980" windowHeight="21840" xr2:uid="{BBE6853E-83EE-46DB-AB5D-CEB4AC5F861C}"/>
   </bookViews>
@@ -803,8 +803,8 @@
   <dimension ref="A1:F120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,7 +874,7 @@
         <v>128</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -910,11 +910,11 @@
       <c r="D5" t="s">
         <v>128</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>129</v>
+      <c r="E5" t="s">
+        <v>128</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -930,11 +930,11 @@
       <c r="D6" t="s">
         <v>128</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>129</v>
+      <c r="E6" t="s">
+        <v>128</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -950,11 +950,11 @@
       <c r="D7" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>129</v>
+      <c r="E7" t="s">
+        <v>128</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -970,11 +970,11 @@
       <c r="D8" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>129</v>
+      <c r="E8" t="s">
+        <v>128</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -990,11 +990,11 @@
       <c r="D9" t="s">
         <v>128</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>129</v>
+      <c r="E9" t="s">
+        <v>128</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1010,11 +1010,11 @@
       <c r="D10" t="s">
         <v>128</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>129</v>
+      <c r="E10" t="s">
+        <v>128</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1030,11 +1030,11 @@
       <c r="D11" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>129</v>
+      <c r="E11" t="s">
+        <v>128</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1050,11 +1050,11 @@
       <c r="D12" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>129</v>
+      <c r="E12" t="s">
+        <v>128</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1231,10 +1231,10 @@
         <v>128</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -3191,7 +3191,7 @@
       </c>
       <c r="E119" s="4">
         <f>SUMIFS($C2:$C118,E2:E118,"=yes")</f>
-        <v>91637</v>
+        <v>105468</v>
       </c>
       <c r="F119" s="4">
         <f>SUMIFS($C2:$C118,F2:F118,"=yes")</f>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="E120" s="5">
         <f>E119/$C119</f>
-        <v>0.26660906046614474</v>
+        <v>0.30684902811357151</v>
       </c>
       <c r="F120" s="5">
         <f>F119/$C119</f>

</xml_diff>

<commit_message>
updated DE progress and dictionary
</commit_message>
<xml_diff>
--- a/designs/i18n-de/i18n-de-progress.xlsx
+++ b/designs/i18n-de/i18n-de-progress.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\heikokue-node-red-designs\designs\i18n-de\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0913CC-B74F-44F4-A60C-E95A01C18E0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D23B05-047B-4739-B553-1E3CB0A99BA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="-120" windowWidth="49980" windowHeight="21840" xr2:uid="{BBE6853E-83EE-46DB-AB5D-CEB4AC5F861C}"/>
   </bookViews>
@@ -803,8 +803,8 @@
   <dimension ref="A1:F120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F113" sqref="F113"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,11 +1070,11 @@
       <c r="D13" t="s">
         <v>128</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>129</v>
+      <c r="E13" t="s">
+        <v>128</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1090,11 +1090,11 @@
       <c r="D14" t="s">
         <v>128</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>129</v>
+      <c r="E14" t="s">
+        <v>128</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1110,11 +1110,11 @@
       <c r="D15" t="s">
         <v>128</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>129</v>
+      <c r="E15" t="s">
+        <v>128</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1130,11 +1130,11 @@
       <c r="D16" t="s">
         <v>128</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>129</v>
+      <c r="E16" t="s">
+        <v>128</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1150,11 +1150,11 @@
       <c r="D17" t="s">
         <v>128</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>129</v>
+      <c r="E17" t="s">
+        <v>128</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1170,11 +1170,11 @@
       <c r="D18" t="s">
         <v>128</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>129</v>
+      <c r="E18" t="s">
+        <v>128</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1190,11 +1190,11 @@
       <c r="D19" t="s">
         <v>128</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>129</v>
+      <c r="E19" t="s">
+        <v>128</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1210,11 +1210,11 @@
       <c r="D20" t="s">
         <v>128</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>129</v>
+      <c r="E20" t="s">
+        <v>128</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1230,11 +1230,11 @@
       <c r="D21" t="s">
         <v>128</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>133</v>
+      <c r="E21" t="s">
+        <v>128</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1250,11 +1250,11 @@
       <c r="D22" t="s">
         <v>128</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>129</v>
+      <c r="E22" t="s">
+        <v>128</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1270,11 +1270,11 @@
       <c r="D23" t="s">
         <v>128</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>129</v>
+      <c r="E23" t="s">
+        <v>128</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1290,11 +1290,11 @@
       <c r="D24" t="s">
         <v>128</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>129</v>
+      <c r="E24" t="s">
+        <v>128</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1310,11 +1310,11 @@
       <c r="D25" t="s">
         <v>128</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>129</v>
+      <c r="E25" t="s">
+        <v>128</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1330,11 +1330,11 @@
       <c r="D26" t="s">
         <v>128</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>129</v>
+      <c r="E26" t="s">
+        <v>128</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1350,11 +1350,11 @@
       <c r="D27" t="s">
         <v>128</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>129</v>
+      <c r="E27" t="s">
+        <v>128</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1370,11 +1370,11 @@
       <c r="D28" t="s">
         <v>128</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>129</v>
+      <c r="E28" t="s">
+        <v>128</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1390,11 +1390,11 @@
       <c r="D29" t="s">
         <v>128</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>129</v>
+      <c r="E29" t="s">
+        <v>128</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1410,11 +1410,11 @@
       <c r="D30" t="s">
         <v>128</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>129</v>
+      <c r="E30" t="s">
+        <v>128</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1430,11 +1430,11 @@
       <c r="D31" t="s">
         <v>128</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>129</v>
+      <c r="E31" t="s">
+        <v>128</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1450,11 +1450,11 @@
       <c r="D32" t="s">
         <v>128</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>129</v>
+      <c r="E32" t="s">
+        <v>128</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1470,11 +1470,11 @@
       <c r="D33" t="s">
         <v>128</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>129</v>
+      <c r="E33" t="s">
+        <v>128</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1490,11 +1490,11 @@
       <c r="D34" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>129</v>
+      <c r="E34" t="s">
+        <v>128</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1510,11 +1510,11 @@
       <c r="D35" t="s">
         <v>128</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>129</v>
+      <c r="E35" t="s">
+        <v>128</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1530,11 +1530,11 @@
       <c r="D36" t="s">
         <v>128</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>129</v>
+      <c r="E36" t="s">
+        <v>128</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1550,11 +1550,11 @@
       <c r="D37" t="s">
         <v>128</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>129</v>
+      <c r="E37" t="s">
+        <v>128</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1570,11 +1570,11 @@
       <c r="D38" t="s">
         <v>128</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>129</v>
+      <c r="E38" t="s">
+        <v>128</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1590,11 +1590,11 @@
       <c r="D39" t="s">
         <v>128</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>129</v>
+      <c r="E39" t="s">
+        <v>128</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1610,11 +1610,11 @@
       <c r="D40" t="s">
         <v>128</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>133</v>
+      <c r="E40" t="s">
+        <v>128</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1633,8 +1633,8 @@
       <c r="E41" t="s">
         <v>128</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>133</v>
+      <c r="F41" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1653,8 +1653,8 @@
       <c r="E42" t="s">
         <v>128</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>133</v>
+      <c r="F42" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1673,8 +1673,8 @@
       <c r="E43" t="s">
         <v>128</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>133</v>
+      <c r="F43" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1693,8 +1693,8 @@
       <c r="E44" t="s">
         <v>128</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>133</v>
+      <c r="F44" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1713,8 +1713,8 @@
       <c r="E45" t="s">
         <v>128</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>133</v>
+      <c r="F45" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1733,8 +1733,8 @@
       <c r="E46" t="s">
         <v>128</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>133</v>
+      <c r="F46" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1753,8 +1753,8 @@
       <c r="E47" t="s">
         <v>128</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>133</v>
+      <c r="F47" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1773,8 +1773,8 @@
       <c r="E48" t="s">
         <v>128</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>133</v>
+      <c r="F48" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1793,8 +1793,8 @@
       <c r="E49" t="s">
         <v>128</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>133</v>
+      <c r="F49" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1813,8 +1813,8 @@
       <c r="E50" t="s">
         <v>128</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>133</v>
+      <c r="F50" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1833,8 +1833,8 @@
       <c r="E51" t="s">
         <v>128</v>
       </c>
-      <c r="F51" s="2" t="s">
-        <v>133</v>
+      <c r="F51" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1853,8 +1853,8 @@
       <c r="E52" t="s">
         <v>128</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>133</v>
+      <c r="F52" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -3191,11 +3191,11 @@
       </c>
       <c r="E119" s="4">
         <f>SUMIFS($C2:$C118,E2:E118,"=yes")</f>
-        <v>105468</v>
+        <v>231288</v>
       </c>
       <c r="F119" s="4">
         <f>SUMIFS($C2:$C118,F2:F118,"=yes")</f>
-        <v>0</v>
+        <v>17095</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3205,11 +3205,11 @@
       </c>
       <c r="E120" s="5">
         <f>E119/$C119</f>
-        <v>0.30684902811357151</v>
+        <v>0.67291024779394437</v>
       </c>
       <c r="F120" s="5">
         <f>F119/$C119</f>
-        <v>0</v>
+        <v>4.9736262521347753E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>